<commit_message>
MASTER: Implement Subjective Evaluation
</commit_message>
<xml_diff>
--- a/doc/Subjective Evaluation (Metadata).xlsx
+++ b/doc/Subjective Evaluation (Metadata).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssimoes\Documents\GitRepos\MMIRMusicRecommender\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidadedecoimbra154-my.sharepoint.com/personal/uc2019217573_student_uc_pt/Documents/Desktop/UNI/Git_Repo/Multimedia TP2/MMIRMusicRecommender/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC0DE14-3A3E-4899-B17C-6DA0543D65BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{0EC0DE14-3A3E-4899-B17C-6DA0543D65BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D010CAA-27AA-4A05-980D-209B5A59D0BE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88C593F1-7AF5-430A-A3F2-E7FE0FF13C9B}"/>
+    <workbookView xWindow="3504" yWindow="696" windowWidth="16572" windowHeight="9420" xr2:uid="{88C593F1-7AF5-430A-A3F2-E7FE0FF13C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -548,13 +551,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -566,18 +576,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="60% - Cor3" xfId="2" builtinId="40"/>
+    <cellStyle name="60% - Accent3" xfId="2" builtinId="40"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Verificar Célula" xfId="1" builtinId="23"/>
   </cellStyles>
   <dxfs count="16">
     <dxf>
@@ -736,7 +739,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1034,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E1B9E6-B0FF-4E99-81BB-013559980CEC}">
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI26" sqref="AI26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,66 +1061,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="14"/>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="12" t="s">
+      <c r="H1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="12" t="s">
+      <c r="M1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="12" t="s">
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="W1" s="5"/>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11" t="s">
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
       <c r="AD1" s="5"/>
     </row>
     <row r="2" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
@@ -1127,8 +1130,8 @@
       <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
@@ -1138,8 +1141,8 @@
       <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
       <c r="M2" s="7" t="s">
         <v>6</v>
       </c>
@@ -1149,8 +1152,8 @@
       <c r="O2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
       <c r="R2" s="7" t="s">
         <v>6</v>
       </c>
@@ -1160,8 +1163,8 @@
       <c r="T2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
       <c r="W2" s="5"/>
       <c r="X2" s="7" t="s">
         <v>6</v>
@@ -1187,54 +1190,62 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="4" t="e">
+      <c r="F3" s="4">
         <f>AVERAGE(C3,D3,E3)</f>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="G3" s="4" t="e">
         <f>STDEV(C3,D3,E3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="4" t="e">
+      <c r="K3" s="4">
         <f>AVERAGE(H3,I3,J3)</f>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="L3" s="4" t="e">
         <f>STDEV(H3,I3,J3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M3" s="1"/>
+      <c r="M3" s="1">
+        <v>3</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="4" t="e">
+      <c r="P3" s="4">
         <f>AVERAGE(M3,N3,O3)</f>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="Q3" s="4" t="e">
         <f>STDEV(M3,N3,O3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R3" s="1"/>
+      <c r="R3" s="1">
+        <v>5</v>
+      </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="U3" s="4" t="e">
+      <c r="U3" s="4">
         <f>AVERAGE(R3,S3,T3)</f>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="V3" s="4" t="e">
         <f>STDEV(R3,S3,T3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W3" s="5"/>
-      <c r="X3" s="4" t="e">
+      <c r="X3" s="4">
         <f t="shared" ref="X3:X22" si="0">AVERAGE(C3,H3,M3,R3)</f>
-        <v>#DIV/0!</v>
+        <v>3.5</v>
       </c>
       <c r="Y3" s="4" t="e">
         <f t="shared" ref="Y3:Y22" si="1">AVERAGE(D3,I3,N3,S3)</f>
@@ -1244,9 +1255,9 @@
         <f t="shared" ref="Z3:Z22" si="2">AVERAGE(E3,J3,O3,T3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA3" s="4" t="e">
+      <c r="AA3" s="4">
         <f t="shared" ref="AA3:AA22" si="3">STDEV(C3,H3,M3,R3)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="AB3" s="4" t="e">
         <f t="shared" ref="AB3:AB22" si="4">STDEV(D3,I3,N3,S3)</f>
@@ -1262,54 +1273,62 @@
       <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="4" t="e">
+      <c r="F4" s="4">
         <f t="shared" ref="F4:F22" si="6">AVERAGE(C4,D4,E4)</f>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="G4" s="4" t="e">
         <f t="shared" ref="G4:G22" si="7">STDEV(C4,D4,E4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="4" t="e">
+      <c r="K4" s="4">
         <f t="shared" ref="K4:K22" si="8">AVERAGE(H4,I4,J4)</f>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="L4" s="4" t="e">
         <f t="shared" ref="L4:L22" si="9">STDEV(H4,I4,J4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1">
+        <v>2</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="4" t="e">
+      <c r="P4" s="4">
         <f t="shared" ref="P4:P22" si="10">AVERAGE(M4,N4,O4)</f>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="4" t="e">
         <f t="shared" ref="Q4:Q22" si="11">STDEV(M4,N4,O4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R4" s="1"/>
+      <c r="R4" s="1">
+        <v>5</v>
+      </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="4" t="e">
+      <c r="U4" s="4">
         <f t="shared" ref="U4:U22" si="12">AVERAGE(R4,S4,T4)</f>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="V4" s="4" t="e">
         <f t="shared" ref="V4:V22" si="13">STDEV(R4,S4,T4)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W4" s="5"/>
-      <c r="X4" s="4" t="e">
+      <c r="X4" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="Y4" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1319,9 +1338,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA4" s="4" t="e">
+      <c r="AA4" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="AB4" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1337,54 +1356,62 @@
       <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="4" t="e">
+      <c r="F5" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="G5" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="4" t="e">
+      <c r="K5" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="L5" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M5" s="1"/>
+      <c r="M5" s="1">
+        <v>4</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="4" t="e">
+      <c r="P5" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="Q5" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R5" s="1"/>
+      <c r="R5" s="1">
+        <v>5</v>
+      </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="4" t="e">
+      <c r="U5" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="V5" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W5" s="5"/>
-      <c r="X5" s="4" t="e">
+      <c r="X5" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4.5</v>
       </c>
       <c r="Y5" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1394,9 +1421,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA5" s="4" t="e">
+      <c r="AA5" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.57735026918962573</v>
       </c>
       <c r="AB5" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1412,54 +1439,62 @@
       <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="4" t="e">
+      <c r="F6" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="G6" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="4" t="e">
+      <c r="K6" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="L6" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="4" t="e">
+      <c r="P6" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R6" s="1"/>
+      <c r="R6" s="1">
+        <v>5</v>
+      </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="4" t="e">
+      <c r="U6" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="V6" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W6" s="5"/>
-      <c r="X6" s="4" t="e">
+      <c r="X6" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="Y6" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1469,9 +1504,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA6" s="4" t="e">
+      <c r="AA6" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
       <c r="AB6" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1487,54 +1522,62 @@
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="4" t="e">
+      <c r="F7" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="4" t="e">
+      <c r="K7" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="L7" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="4" t="e">
+      <c r="P7" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="Q7" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R7" s="1"/>
+      <c r="R7" s="1">
+        <v>5</v>
+      </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="4" t="e">
+      <c r="U7" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="V7" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W7" s="5"/>
-      <c r="X7" s="4" t="e">
+      <c r="X7" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="Y7" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1544,9 +1587,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA7" s="4" t="e">
+      <c r="AA7" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
       <c r="AB7" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1562,54 +1605,62 @@
       <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="4" t="e">
+      <c r="F8" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="4" t="e">
+      <c r="K8" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="L8" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="1"/>
+      <c r="M8" s="1">
+        <v>4</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="4" t="e">
+      <c r="P8" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="Q8" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R8" s="1"/>
+      <c r="R8" s="1">
+        <v>1</v>
+      </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="4" t="e">
+      <c r="U8" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="V8" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W8" s="5"/>
-      <c r="X8" s="4" t="e">
+      <c r="X8" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.75</v>
       </c>
       <c r="Y8" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1619,9 +1670,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA8" s="4" t="e">
+      <c r="AA8" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
       <c r="AB8" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1637,54 +1688,62 @@
       <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="4" t="e">
+      <c r="F9" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="G9" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="4" t="e">
+      <c r="K9" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="L9" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M9" s="1"/>
+      <c r="M9" s="1">
+        <v>4</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="4" t="e">
+      <c r="P9" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="Q9" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="1"/>
+      <c r="R9" s="1">
+        <v>5</v>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="4" t="e">
+      <c r="U9" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="V9" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W9" s="5"/>
-      <c r="X9" s="4" t="e">
+      <c r="X9" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="Y9" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1694,9 +1753,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA9" s="4" t="e">
+      <c r="AA9" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.9574271077563381</v>
       </c>
       <c r="AB9" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1712,54 +1771,62 @@
       <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="4" t="e">
+      <c r="F10" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="G10" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="4" t="e">
+      <c r="K10" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="L10" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M10" s="1"/>
+      <c r="M10" s="1">
+        <v>3</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="4" t="e">
+      <c r="P10" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R10" s="1"/>
+      <c r="R10" s="1">
+        <v>1</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
-      <c r="U10" s="4" t="e">
+      <c r="U10" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="V10" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W10" s="5"/>
-      <c r="X10" s="4" t="e">
+      <c r="X10" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.75</v>
       </c>
       <c r="Y10" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1769,9 +1836,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA10" s="4" t="e">
+      <c r="AA10" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.9574271077563381</v>
       </c>
       <c r="AB10" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1787,54 +1854,62 @@
       <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="4" t="e">
+      <c r="F11" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G11" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>5</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="4" t="e">
+      <c r="K11" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="L11" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M11" s="1"/>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="4" t="e">
+      <c r="P11" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R11" s="1"/>
+      <c r="R11" s="1">
+        <v>1</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
-      <c r="U11" s="4" t="e">
+      <c r="U11" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="V11" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W11" s="5"/>
-      <c r="X11" s="4" t="e">
+      <c r="X11" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="Y11" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1844,9 +1919,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA11" s="4" t="e">
+      <c r="AA11" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="AB11" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1862,54 +1937,62 @@
       <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="4" t="e">
+      <c r="F12" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="4" t="e">
+      <c r="K12" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="L12" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M12" s="1"/>
+      <c r="M12" s="1">
+        <v>4</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="4" t="e">
+      <c r="P12" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="Q12" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R12" s="1"/>
+      <c r="R12" s="1">
+        <v>1</v>
+      </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="4" t="e">
+      <c r="U12" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="V12" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W12" s="5"/>
-      <c r="X12" s="4" t="e">
+      <c r="X12" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.25</v>
       </c>
       <c r="Y12" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1919,9 +2002,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA12" s="4" t="e">
+      <c r="AA12" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.2583057392117916</v>
       </c>
       <c r="AB12" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1937,54 +2020,62 @@
       <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="4" t="e">
+      <c r="F13" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G13" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="4" t="e">
+      <c r="K13" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="L13" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="1"/>
+      <c r="M13" s="1">
+        <v>4</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="4" t="e">
+      <c r="P13" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="Q13" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R13" s="1"/>
+      <c r="R13" s="1">
+        <v>1</v>
+      </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="4" t="e">
+      <c r="U13" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="V13" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W13" s="5"/>
-      <c r="X13" s="4" t="e">
+      <c r="X13" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="Y13" s="4" t="e">
         <f t="shared" si="1"/>
@@ -1994,9 +2085,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA13" s="4" t="e">
+      <c r="AA13" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="AB13" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2012,54 +2103,62 @@
       <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="4" t="e">
+      <c r="F14" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G14" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>4</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="4" t="e">
+      <c r="K14" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="L14" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M14" s="1"/>
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="4" t="e">
+      <c r="P14" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R14" s="1"/>
+      <c r="R14" s="1">
+        <v>1</v>
+      </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
-      <c r="U14" s="4" t="e">
+      <c r="U14" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="V14" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W14" s="5"/>
-      <c r="X14" s="4" t="e">
+      <c r="X14" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.75</v>
       </c>
       <c r="Y14" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2069,9 +2168,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA14" s="4" t="e">
+      <c r="AA14" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
       <c r="AB14" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2087,54 +2186,62 @@
       <c r="B15" s="2">
         <v>13</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="4" t="e">
+      <c r="F15" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="G15" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1">
+        <v>4</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="4" t="e">
+      <c r="K15" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="L15" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M15" s="1"/>
+      <c r="M15" s="1">
+        <v>3</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="4" t="e">
+      <c r="P15" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="Q15" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R15" s="1"/>
+      <c r="R15" s="1">
+        <v>1</v>
+      </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
-      <c r="U15" s="4" t="e">
+      <c r="U15" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="V15" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W15" s="5"/>
-      <c r="X15" s="4" t="e">
+      <c r="X15" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.5</v>
       </c>
       <c r="Y15" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2144,9 +2251,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA15" s="4" t="e">
+      <c r="AA15" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.2909944487358056</v>
       </c>
       <c r="AB15" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2162,54 +2269,62 @@
       <c r="B16" s="2">
         <v>14</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="4" t="e">
+      <c r="F16" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="4" t="e">
+      <c r="K16" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="L16" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M16" s="1"/>
+      <c r="M16" s="1">
+        <v>2</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="4" t="e">
+      <c r="P16" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R16" s="1"/>
+      <c r="R16" s="1">
+        <v>4</v>
+      </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
-      <c r="U16" s="4" t="e">
+      <c r="U16" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="V16" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W16" s="5"/>
-      <c r="X16" s="4" t="e">
+      <c r="X16" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2.75</v>
       </c>
       <c r="Y16" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2219,9 +2334,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA16" s="4" t="e">
+      <c r="AA16" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
       <c r="AB16" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2237,54 +2352,62 @@
       <c r="B17" s="2">
         <v>15</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="4" t="e">
+      <c r="F17" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="G17" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="4" t="e">
+      <c r="K17" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="L17" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M17" s="1"/>
+      <c r="M17" s="1">
+        <v>2</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="4" t="e">
+      <c r="P17" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="Q17" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R17" s="1"/>
+      <c r="R17" s="1">
+        <v>5</v>
+      </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="4" t="e">
+      <c r="U17" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="V17" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W17" s="5"/>
-      <c r="X17" s="4" t="e">
+      <c r="X17" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.25</v>
       </c>
       <c r="Y17" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2294,9 +2417,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA17" s="4" t="e">
+      <c r="AA17" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.2583057392117916</v>
       </c>
       <c r="AB17" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2312,54 +2435,62 @@
       <c r="B18" s="2">
         <v>16</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="4" t="e">
+      <c r="F18" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="G18" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1">
+        <v>3</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="4" t="e">
+      <c r="K18" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="L18" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M18" s="1"/>
+      <c r="M18" s="1">
+        <v>5</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="4" t="e">
+      <c r="P18" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="Q18" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R18" s="1"/>
+      <c r="R18" s="1">
+        <v>5</v>
+      </c>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
-      <c r="U18" s="4" t="e">
+      <c r="U18" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="V18" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W18" s="5"/>
-      <c r="X18" s="4" t="e">
+      <c r="X18" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="Y18" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2369,9 +2500,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA18" s="4" t="e">
+      <c r="AA18" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
       <c r="AB18" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2387,54 +2518,62 @@
       <c r="B19" s="2">
         <v>17</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="4" t="e">
+      <c r="F19" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G19" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1">
+        <v>3</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="4" t="e">
+      <c r="K19" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="L19" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M19" s="1"/>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="4" t="e">
+      <c r="P19" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R19" s="1"/>
+      <c r="R19" s="1">
+        <v>2</v>
+      </c>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
-      <c r="U19" s="4" t="e">
+      <c r="U19" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="V19" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W19" s="5"/>
-      <c r="X19" s="4" t="e">
+      <c r="X19" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.75</v>
       </c>
       <c r="Y19" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2444,9 +2583,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA19" s="4" t="e">
+      <c r="AA19" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.9574271077563381</v>
       </c>
       <c r="AB19" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2462,54 +2601,62 @@
       <c r="B20" s="2">
         <v>18</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="4" t="e">
+      <c r="F20" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G20" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="4" t="e">
+      <c r="K20" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="L20" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M20" s="1"/>
+      <c r="M20" s="1">
+        <v>2</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="4" t="e">
+      <c r="P20" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="Q20" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R20" s="1"/>
+      <c r="R20" s="1">
+        <v>2</v>
+      </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
-      <c r="U20" s="4" t="e">
+      <c r="U20" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="V20" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W20" s="5"/>
-      <c r="X20" s="4" t="e">
+      <c r="X20" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.75</v>
       </c>
       <c r="Y20" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2519,9 +2666,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA20" s="4" t="e">
+      <c r="AA20" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="AB20" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2537,54 +2684,62 @@
       <c r="B21" s="2">
         <v>19</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="4" t="e">
+      <c r="F21" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
       <c r="G21" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1">
+        <v>5</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="4" t="e">
+      <c r="K21" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="L21" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M21" s="1"/>
+      <c r="M21" s="1">
+        <v>4</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="4" t="e">
+      <c r="P21" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="Q21" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R21" s="1"/>
+      <c r="R21" s="1">
+        <v>4</v>
+      </c>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
-      <c r="U21" s="4" t="e">
+      <c r="U21" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="V21" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W21" s="5"/>
-      <c r="X21" s="4" t="e">
+      <c r="X21" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="Y21" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2594,9 +2749,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA21" s="4" t="e">
+      <c r="AA21" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.2583057392117916</v>
       </c>
       <c r="AB21" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2612,54 +2767,62 @@
       <c r="B22" s="3">
         <v>20</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="4" t="e">
+      <c r="F22" s="4">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="G22" s="4" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>4</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="4" t="e">
+      <c r="K22" s="4">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="L22" s="4" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M22" s="1"/>
+      <c r="M22" s="1">
+        <v>4</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="4" t="e">
+      <c r="P22" s="4">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="Q22" s="4" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R22" s="1"/>
+      <c r="R22" s="1">
+        <v>4</v>
+      </c>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
-      <c r="U22" s="4" t="e">
+      <c r="U22" s="4">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="V22" s="4" t="e">
         <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W22" s="5"/>
-      <c r="X22" s="4" t="e">
+      <c r="X22" s="4">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="Y22" s="4" t="e">
         <f t="shared" si="1"/>
@@ -2669,9 +2832,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA22" s="4" t="e">
+      <c r="AA22" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="AB22" s="4" t="e">
         <f t="shared" si="4"/>
@@ -2685,44 +2848,44 @@
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="6" t="e">
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="6">
         <f>COUNTIF(F3:F22,"&gt;="&amp;G27) / COUNT(F3:F22) * 100</f>
-        <v>#DIV/0!</v>
+        <v>35</v>
       </c>
       <c r="G23" s="5"/>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="6" t="e">
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="6">
         <f>COUNTIF(K3:K22,"&gt;="&amp;G27) / COUNT(K3:K22) * 100</f>
-        <v>#DIV/0!</v>
+        <v>65</v>
       </c>
       <c r="L23" s="5"/>
-      <c r="M23" s="11" t="s">
+      <c r="M23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="6" t="e">
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="6">
         <f>COUNTIF(P3:P22,"&gt;="&amp;G27) / COUNT(P3:P22) * 100</f>
-        <v>#DIV/0!</v>
+        <v>65</v>
       </c>
       <c r="Q23" s="5"/>
-      <c r="R23" s="11" t="s">
+      <c r="R23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="6" t="e">
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="6">
         <f>COUNTIF(U3:U22,"&gt;="&amp;G27) / COUNT(U3:U22) * 100</f>
-        <v>#DIV/0!</v>
+        <v>55.000000000000007</v>
       </c>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
@@ -2735,41 +2898,41 @@
       <c r="AD23" s="5"/>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="8">
         <v>2.5</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="19"/>
-      <c r="X27" s="13" t="s">
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="Y27" s="13"/>
+      <c r="Y27" s="14"/>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B28" s="9"/>
@@ -2778,32 +2941,32 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="I28" s="19" t="s">
+      <c r="I28" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19" t="s">
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19" t="s">
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-      <c r="W28" s="19"/>
-      <c r="X28" s="19" t="s">
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+      <c r="W28" s="11"/>
+      <c r="X28" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="Y28" s="19"/>
-      <c r="Z28" s="19"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
@@ -2816,32 +2979,32 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="I29" s="19" t="s">
+      <c r="I29" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19" t="s">
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19" t="s">
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="T29" s="19"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="19"/>
-      <c r="W29" s="19"/>
-      <c r="X29" s="19" t="s">
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+      <c r="W29" s="11"/>
+      <c r="X29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="Y29" s="19"/>
-      <c r="Z29" s="19"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
@@ -2854,32 +3017,32 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="I30" s="19" t="s">
+      <c r="I30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19" t="s">
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19" t="s">
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-      <c r="W30" s="19"/>
-      <c r="X30" s="19" t="s">
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="Y30" s="19"/>
-      <c r="Z30" s="19"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
@@ -2892,495 +3055,483 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="I31" s="19" t="s">
+      <c r="I31" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19" t="s">
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19" t="s">
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="19"/>
-      <c r="X31" s="19" t="s">
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="Y31" s="19"/>
-      <c r="Z31" s="19"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19" t="s">
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19" t="s">
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="19" t="s">
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="Y32" s="19"/>
-      <c r="Z32" s="19"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
     </row>
     <row r="33" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I33" s="19" t="s">
+      <c r="I33" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19" t="s">
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19" t="s">
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="19"/>
-      <c r="X33" s="19" t="s">
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="Y33" s="19"/>
-      <c r="Z33" s="19"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="11"/>
     </row>
     <row r="34" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I34" s="19" t="s">
+      <c r="I34" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19" t="s">
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19" t="s">
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19"/>
-      <c r="X34" s="19" t="s">
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="Y34" s="19"/>
-      <c r="Z34" s="19"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
     </row>
     <row r="35" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I35" s="19" t="s">
+      <c r="I35" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19" t="s">
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19" t="s">
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="W35" s="19"/>
-      <c r="X35" s="19" t="s">
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="Y35" s="19"/>
-      <c r="Z35" s="19"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
     </row>
     <row r="36" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I36" s="19" t="s">
+      <c r="I36" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19" t="s">
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19" t="s">
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
-      <c r="V36" s="19"/>
-      <c r="W36" s="19"/>
-      <c r="X36" s="19" t="s">
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="Y36" s="19"/>
-      <c r="Z36" s="19"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
     </row>
     <row r="37" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I37" s="19" t="s">
+      <c r="I37" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19" t="s">
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19" t="s">
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19" t="s">
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="Y37" s="19"/>
-      <c r="Z37" s="19"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
     </row>
     <row r="38" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I38" s="19" t="s">
+      <c r="I38" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19" t="s">
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19" t="s">
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19" t="s">
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="Y38" s="19"/>
-      <c r="Z38" s="19"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
     </row>
     <row r="39" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I39" s="19" t="s">
+      <c r="I39" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19" t="s">
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
-      <c r="S39" s="19" t="s">
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="T39" s="19"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="19"/>
-      <c r="W39" s="19"/>
-      <c r="X39" s="19" t="s">
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="Y39" s="19"/>
-      <c r="Z39" s="19"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
     </row>
     <row r="40" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I40" s="19" t="s">
+      <c r="I40" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19" t="s">
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
-      <c r="R40" s="19"/>
-      <c r="S40" s="19" t="s">
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="T40" s="19"/>
-      <c r="U40" s="19"/>
-      <c r="V40" s="19"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="19" t="s">
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Y40" s="19"/>
-      <c r="Z40" s="19"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
     </row>
     <row r="41" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I41" s="19" t="s">
+      <c r="I41" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19" t="s">
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19" t="s">
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19" t="s">
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="Y41" s="19"/>
-      <c r="Z41" s="19"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
     </row>
     <row r="42" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I42" s="19" t="s">
+      <c r="I42" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19" t="s">
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19" t="s">
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19" t="s">
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="Y42" s="19"/>
-      <c r="Z42" s="19"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="11"/>
     </row>
     <row r="43" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I43" s="19" t="s">
+      <c r="I43" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19" t="s">
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
-      <c r="S43" s="19" t="s">
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="T43" s="19"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="19" t="s">
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="Y43" s="19"/>
-      <c r="Z43" s="19"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
     </row>
     <row r="44" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I44" s="19" t="s">
+      <c r="I44" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19" t="s">
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19" t="s">
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19" t="s">
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="Y44" s="19"/>
-      <c r="Z44" s="19"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
     </row>
     <row r="45" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I45" s="19" t="s">
+      <c r="I45" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19" t="s">
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19" t="s">
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19" t="s">
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="Y45" s="19"/>
-      <c r="Z45" s="19"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
     </row>
     <row r="46" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I46" s="19" t="s">
+      <c r="I46" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19" t="s">
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
-      <c r="S46" s="19" t="s">
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19" t="s">
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
+      <c r="X46" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="Y46" s="19"/>
-      <c r="Z46" s="19"/>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="11"/>
     </row>
     <row r="47" spans="9:26" x14ac:dyDescent="0.3">
-      <c r="I47" s="19" t="s">
+      <c r="I47" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19" t="s">
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="O47" s="19"/>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="19"/>
-      <c r="R47" s="19"/>
-      <c r="S47" s="19" t="s">
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="T47" s="19"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="19"/>
-      <c r="X47" s="19" t="s">
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="Y47" s="19"/>
-      <c r="Z47" s="19"/>
+      <c r="Y47" s="11"/>
+      <c r="Z47" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="C1:E1"/>
     <mergeCell ref="X1:Z1"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="R23:T23"/>
@@ -3393,6 +3544,18 @@
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="R1:T1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="B27:F27"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C3:E22">

</xml_diff>